<commit_message>
testing out the generation of new json schemas and updating records accordingly.
</commit_message>
<xml_diff>
--- a/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
+++ b/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/tox_Dataharmonier/web/templates/mass_spec_metabolomics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/ToxRSCat/templates/mass_spec_metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="371" documentId="13_ncr:1_{312CE87D-C60B-3744-983C-44476127223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E99E7749-DCF7-4CAA-99C3-EB61F11D34F1}"/>
+  <xr:revisionPtr revIDLastSave="378" documentId="13_ncr:1_{312CE87D-C60B-3744-983C-44476127223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C03CDC85-96E4-456E-9219-DEA53D265955}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="24915" windowHeight="12735" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_slots" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="132">
   <si>
     <t>description</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>obo:OBI:0000021</t>
-  </si>
-  <si>
-    <t>FCS File name (must end in .FCS)</t>
   </si>
   <si>
     <t>TransformationPurpose</t>
@@ -523,12 +520,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -863,18 +859,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="18" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -930,44 +924,44 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
       </c>
       <c r="L2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O2" t="b">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>26</v>
       </c>
       <c r="R2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -978,26 +972,26 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" t="b">
         <v>1</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -1008,25 +1002,24 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" t="s">
-        <v>96</v>
-      </c>
-      <c r="O4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
@@ -1037,7 +1030,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -1047,11 +1040,11 @@
         <v>1</v>
       </c>
       <c r="Q5" s="1"/>
-      <c r="R5" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1059,7 +1052,7 @@
         <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -1077,10 +1070,10 @@
         <v>26</v>
       </c>
       <c r="R6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1088,7 +1081,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
@@ -1109,10 +1102,10 @@
         <v>26</v>
       </c>
       <c r="R7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1138,69 +1131,69 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
         <v>60</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
         <v>61</v>
       </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L9" t="s">
-        <v>103</v>
-      </c>
-      <c r="O9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" t="s">
+        <v>105</v>
+      </c>
+      <c r="N10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
         <v>62</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L10" t="s">
-        <v>106</v>
-      </c>
-      <c r="N10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>63</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="K11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>34</v>
@@ -1212,201 +1205,201 @@
         <v>35</v>
       </c>
       <c r="L12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" t="s">
+        <v>102</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" t="s">
+        <v>105</v>
+      </c>
+      <c r="N15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C16" t="s">
         <v>65</v>
       </c>
-      <c r="E13" t="s">
-        <v>23</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
+        <v>66</v>
+      </c>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" t="s">
+        <v>108</v>
+      </c>
+      <c r="R17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>73</v>
-      </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" t="s">
-        <v>103</v>
-      </c>
-      <c r="O14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" t="s">
+        <v>113</v>
+      </c>
+      <c r="R20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
         <v>74</v>
       </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="L15" t="s">
-        <v>106</v>
-      </c>
-      <c r="N15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" t="s">
-        <v>67</v>
-      </c>
-      <c r="O16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" t="s">
-        <v>109</v>
-      </c>
-      <c r="R17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" t="s">
-        <v>114</v>
-      </c>
-      <c r="R20" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>75</v>
       </c>
-      <c r="C21" t="s">
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" t="s">
+        <v>102</v>
+      </c>
+      <c r="O21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" t="s">
         <v>76</v>
       </c>
-      <c r="E21" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" t="s">
-        <v>103</v>
-      </c>
-      <c r="O21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
       <c r="E22" t="s">
         <v>23</v>
       </c>
       <c r="L22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N22" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1423,11 +1416,11 @@
         <v>40</v>
       </c>
       <c r="L23" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1441,22 +1434,22 @@
         <v>27</v>
       </c>
       <c r="K24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O24" t="b">
         <v>1</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="P24" t="s">
         <v>39</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="Q24" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1464,25 +1457,25 @@
         <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" t="s">
         <v>27</v>
       </c>
       <c r="K25" t="s">
+        <v>120</v>
+      </c>
+      <c r="L25" t="s">
+        <v>129</v>
+      </c>
+      <c r="P25" t="s">
         <v>121</v>
       </c>
-      <c r="L25" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>122</v>
-      </c>
-      <c r="R25" s="2" t="s">
+      <c r="Q25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1490,22 +1483,22 @@
         <v>36</v>
       </c>
       <c r="C26" t="s">
+        <v>116</v>
+      </c>
+      <c r="E26" t="s">
+        <v>23</v>
+      </c>
+      <c r="L26" t="s">
         <v>117</v>
       </c>
-      <c r="E26" t="s">
-        <v>23</v>
-      </c>
-      <c r="L26" t="s">
+      <c r="P26" t="s">
         <v>118</v>
       </c>
-      <c r="Q26" t="s">
-        <v>119</v>
-      </c>
-      <c r="R26" s="2" t="s">
+      <c r="Q26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1513,56 +1506,46 @@
         <v>36</v>
       </c>
       <c r="C27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E27" t="s">
+        <v>23</v>
+      </c>
+      <c r="L27" t="s">
         <v>123</v>
       </c>
-      <c r="E27" t="s">
-        <v>23</v>
-      </c>
-      <c r="L27" t="s">
+      <c r="P27" t="s">
         <v>124</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="Q27" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" t="s">
         <v>125</v>
       </c>
-      <c r="R27" s="2" t="s">
+      <c r="P28" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="R28" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1570,22 +1553,22 @@
         <v>41</v>
       </c>
       <c r="C29" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" t="s">
         <v>102</v>
       </c>
-      <c r="E29" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29" t="s">
+      <c r="P29" t="s">
         <v>103</v>
-      </c>
-      <c r="P29" t="s">
-        <v>104</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1593,22 +1576,22 @@
         <v>41</v>
       </c>
       <c r="C30" t="s">
+        <v>104</v>
+      </c>
+      <c r="E30" t="s">
+        <v>23</v>
+      </c>
+      <c r="L30" t="s">
         <v>105</v>
       </c>
-      <c r="E30" t="s">
-        <v>23</v>
-      </c>
-      <c r="L30" t="s">
+      <c r="P30" t="s">
         <v>106</v>
-      </c>
-      <c r="P30" t="s">
-        <v>107</v>
       </c>
       <c r="Q30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1616,22 +1599,19 @@
         <v>41</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
         <v>23</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="P31" t="s">
         <v>42</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="Q31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1654,7 +1634,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" t="s">
         <v>23</v>
@@ -1668,13 +1648,13 @@
         <v>41</v>
       </c>
       <c r="C34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
         <v>23</v>
       </c>
       <c r="L34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -1685,13 +1665,13 @@
         <v>41</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
         <v>23</v>
       </c>
       <c r="L35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -1702,7 +1682,7 @@
         <v>41</v>
       </c>
       <c r="C36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E36" t="s">
         <v>23</v>
@@ -1716,7 +1696,7 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
         <v>23</v>
@@ -1724,13 +1704,13 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
         <v>78</v>
-      </c>
-      <c r="B38" t="s">
-        <v>82</v>
-      </c>
-      <c r="C38" t="s">
-        <v>79</v>
       </c>
       <c r="E38" t="s">
         <v>23</v>
@@ -1744,13 +1724,13 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" t="s">
         <v>23</v>
@@ -1761,13 +1741,13 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" t="s">
         <v>23</v>
@@ -1775,13 +1755,13 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
         <v>82</v>
-      </c>
-      <c r="C41" t="s">
-        <v>83</v>
       </c>
       <c r="E41" t="s">
         <v>23</v>
@@ -1789,13 +1769,13 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E42" t="s">
         <v>23</v>
@@ -1803,13 +1783,13 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E43" t="s">
         <v>23</v>
@@ -1819,16 +1799,16 @@
   <hyperlinks>
     <hyperlink ref="Q6:Q8" r:id="rId1" display="http://purl.obolibrary.org/obo/" xr:uid="{4060DE50-60AB-401F-954D-1314EDCB624C}"/>
     <hyperlink ref="R23:R24" r:id="rId2" display="http://purl.obolibrary.org/obo/" xr:uid="{307762AB-2E7A-47CD-8D3D-7CE78C823F45}"/>
-    <hyperlink ref="R31" r:id="rId3" xr:uid="{33297E6C-E637-4D6A-A0BC-581B2507D525}"/>
+    <hyperlink ref="Q31" r:id="rId3" xr:uid="{33297E6C-E637-4D6A-A0BC-581B2507D525}"/>
     <hyperlink ref="Q2" r:id="rId4" xr:uid="{C1B63C4C-27AD-4E22-8185-5796673CA3AA}"/>
-    <hyperlink ref="R24" r:id="rId5" xr:uid="{08A2F3B9-823C-45C0-969D-0358973D2F16}"/>
+    <hyperlink ref="Q24" r:id="rId5" xr:uid="{08A2F3B9-823C-45C0-969D-0358973D2F16}"/>
     <hyperlink ref="Q29:Q30" r:id="rId6" display="http://purl.obolibrary.org/obo/" xr:uid="{28F37213-D6B5-4C09-8A96-760662AD4884}"/>
     <hyperlink ref="Q29" r:id="rId7" xr:uid="{B0089BD3-5D37-41E4-B827-A728BDB04015}"/>
     <hyperlink ref="Q30" r:id="rId8" xr:uid="{6659EEB8-2061-4ACA-96F4-FD3D15C14968}"/>
-    <hyperlink ref="R26" r:id="rId9" xr:uid="{03F15CA4-4CC8-4E5F-95F9-1B10B541366A}"/>
-    <hyperlink ref="R25" r:id="rId10" xr:uid="{817B7841-B808-4C84-9F77-6406FBC56312}"/>
-    <hyperlink ref="R27" r:id="rId11" xr:uid="{F4AF0096-9932-4C1C-BF5B-FBF5C8F5ACC1}"/>
-    <hyperlink ref="R28" r:id="rId12" xr:uid="{0637E511-30ED-42FB-8DEA-71F67A856866}"/>
+    <hyperlink ref="Q26" r:id="rId9" xr:uid="{03F15CA4-4CC8-4E5F-95F9-1B10B541366A}"/>
+    <hyperlink ref="Q25" r:id="rId10" xr:uid="{817B7841-B808-4C84-9F77-6406FBC56312}"/>
+    <hyperlink ref="Q27" r:id="rId11" xr:uid="{F4AF0096-9932-4C1C-BF5B-FBF5C8F5ACC1}"/>
+    <hyperlink ref="Q28" r:id="rId12" xr:uid="{0637E511-30ED-42FB-8DEA-71F67A856866}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -1868,19 +1848,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>89</v>
       </c>
-      <c r="C2" t="s">
-        <v>90</v>
-      </c>
       <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upgrade miaca, miflowcyt, meta_spec...
</commit_message>
<xml_diff>
--- a/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
+++ b/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/tox_Dataharmonier/web/templates/mass_spec_metabolomics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/mass_spec_metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="371" documentId="13_ncr:1_{312CE87D-C60B-3744-983C-44476127223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E99E7749-DCF7-4CAA-99C3-EB61F11D34F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068CA00F-B5AB-C34E-9C32-7FCEFDD8A366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_slots" sheetId="1" r:id="rId1"/>
@@ -523,12 +523,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -865,16 +873,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
   <dimension ref="A1:S43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="J37" zoomScale="94" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="18" width="21" customWidth="1"/>
+    <col min="1" max="10" width="21" customWidth="1"/>
+    <col min="11" max="15" width="21" style="5" customWidth="1"/>
+    <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="32.1640625" customWidth="1"/>
+    <col min="18" max="18" width="32" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -905,19 +917,19 @@
       <c r="J1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="N1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -926,11 +938,11 @@
       <c r="Q1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -943,10 +955,10 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="O2" t="b">
+      <c r="O2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P2" t="s">
@@ -955,11 +967,11 @@
       <c r="Q2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="170" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -976,20 +988,20 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" t="s">
+      <c r="K3" s="4"/>
+      <c r="L3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" t="b">
+      <c r="N3" s="4"/>
+      <c r="O3" s="5" t="b">
         <v>1</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="170" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -1006,19 +1018,19 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" t="s">
+      <c r="K4" s="4"/>
+      <c r="L4" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="O4" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" s="4" t="s">
+      <c r="O4" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>99</v>
       </c>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -1035,23 +1047,23 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" t="s">
+      <c r="K5" s="4"/>
+      <c r="L5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="M5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="1"/>
-      <c r="O5" t="b">
+      <c r="M5" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="N5" s="4"/>
+      <c r="O5" s="5" t="b">
         <v>1</v>
       </c>
       <c r="Q5" s="1"/>
-      <c r="R5" s="4" t="s">
+      <c r="R5" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -1064,10 +1076,10 @@
       <c r="E6" t="s">
         <v>23</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="N6" t="b">
+      <c r="N6" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P6" t="s">
@@ -1076,11 +1088,11 @@
       <c r="Q6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1096,10 +1108,10 @@
       <c r="J7" t="b">
         <v>1</v>
       </c>
-      <c r="L7" t="s">
+      <c r="L7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="O7" t="b">
+      <c r="O7" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P7" t="s">
@@ -1108,11 +1120,11 @@
       <c r="Q7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -1125,10 +1137,10 @@
       <c r="E8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="N8" t="b">
+      <c r="N8" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P8" t="s">
@@ -1138,7 +1150,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1151,14 +1163,14 @@
       <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L9" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="O9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O9" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1171,14 +1183,14 @@
       <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L10" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N10" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="404" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1191,11 +1203,11 @@
       <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1208,14 +1220,14 @@
       <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1228,11 +1240,11 @@
       <c r="E13" t="s">
         <v>23</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1245,14 +1257,14 @@
       <c r="E14" t="s">
         <v>23</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="O14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O14" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1265,14 +1277,14 @@
       <c r="E15" t="s">
         <v>23</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N15" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1285,14 +1297,14 @@
       <c r="E16" t="s">
         <v>23</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="O16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O16" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1305,14 +1317,14 @@
       <c r="E17" t="s">
         <v>23</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L17" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1325,11 +1337,11 @@
       <c r="E18" t="s">
         <v>23</v>
       </c>
-      <c r="L18" t="s">
+      <c r="L18" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1342,11 +1354,11 @@
       <c r="E19" t="s">
         <v>23</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -1359,14 +1371,14 @@
       <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1379,14 +1391,14 @@
       <c r="E21" t="s">
         <v>23</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="O21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O21" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -1399,14 +1411,14 @@
       <c r="E22" t="s">
         <v>23</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="N22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N22" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -1419,15 +1431,15 @@
       <c r="E23" t="s">
         <v>27</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L23" t="s">
+      <c r="L23" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="R23" s="2"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R23" s="6"/>
+    </row>
+    <row r="24" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1440,23 +1452,23 @@
       <c r="E24" t="s">
         <v>27</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K24" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L24" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="O24" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q24" t="s">
+      <c r="O24" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P24" t="s">
         <v>39</v>
       </c>
-      <c r="R24" s="2" t="s">
+      <c r="Q24" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1469,20 +1481,20 @@
       <c r="E25" t="s">
         <v>27</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="P25" t="s">
         <v>122</v>
       </c>
-      <c r="R25" s="2" t="s">
+      <c r="Q25" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>33</v>
       </c>
@@ -1495,17 +1507,17 @@
       <c r="E26" t="s">
         <v>23</v>
       </c>
-      <c r="L26" t="s">
+      <c r="L26" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="P26" t="s">
         <v>119</v>
       </c>
-      <c r="R26" s="2" t="s">
+      <c r="Q26" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1518,51 +1530,41 @@
       <c r="E27" t="s">
         <v>23</v>
       </c>
-      <c r="L27" t="s">
+      <c r="L27" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="P27" t="s">
         <v>125</v>
       </c>
-      <c r="R27" s="2" t="s">
+      <c r="Q27" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" t="s">
         <v>127</v>
       </c>
       <c r="D28" s="1"/>
-      <c r="E28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="4" t="s">
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="M28" s="4"/>
-      <c r="N28" s="4"/>
-      <c r="O28" s="4"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4" t="s">
+      <c r="P28" t="s">
         <v>128</v>
       </c>
-      <c r="R28" s="2" t="s">
+      <c r="Q28" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1575,7 +1577,7 @@
       <c r="E29" t="s">
         <v>23</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L29" s="5" t="s">
         <v>103</v>
       </c>
       <c r="P29" t="s">
@@ -1585,7 +1587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>33</v>
       </c>
@@ -1598,7 +1600,7 @@
       <c r="E30" t="s">
         <v>23</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L30" s="5" t="s">
         <v>106</v>
       </c>
       <c r="P30" t="s">
@@ -1608,7 +1610,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1621,17 +1623,17 @@
       <c r="E31" t="s">
         <v>23</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="P31" t="s">
         <v>42</v>
       </c>
-      <c r="R31" s="2" t="s">
+      <c r="Q31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="S31" t="s">
+      <c r="R31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1644,9 +1646,9 @@
       <c r="E32" t="s">
         <v>23</v>
       </c>
-      <c r="R32" s="2"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R32" s="6"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -1660,7 +1662,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" ht="136" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1673,11 +1675,11 @@
       <c r="E34" t="s">
         <v>23</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L34" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="187" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1690,11 +1692,11 @@
       <c r="E35" t="s">
         <v>23</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L35" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1708,7 +1710,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -1722,7 +1724,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1735,14 +1737,14 @@
       <c r="E38" t="s">
         <v>23</v>
       </c>
-      <c r="M38" t="b">
-        <v>1</v>
-      </c>
-      <c r="O38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M38" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="O38" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>78</v>
       </c>
@@ -1755,11 +1757,11 @@
       <c r="E39" t="s">
         <v>23</v>
       </c>
-      <c r="N39" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N39" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>78</v>
       </c>
@@ -1787,7 +1789,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>78</v>
       </c>
@@ -1801,7 +1803,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -1819,16 +1821,16 @@
   <hyperlinks>
     <hyperlink ref="Q6:Q8" r:id="rId1" display="http://purl.obolibrary.org/obo/" xr:uid="{4060DE50-60AB-401F-954D-1314EDCB624C}"/>
     <hyperlink ref="R23:R24" r:id="rId2" display="http://purl.obolibrary.org/obo/" xr:uid="{307762AB-2E7A-47CD-8D3D-7CE78C823F45}"/>
-    <hyperlink ref="R31" r:id="rId3" xr:uid="{33297E6C-E637-4D6A-A0BC-581B2507D525}"/>
+    <hyperlink ref="Q31" r:id="rId3" xr:uid="{33297E6C-E637-4D6A-A0BC-581B2507D525}"/>
     <hyperlink ref="Q2" r:id="rId4" xr:uid="{C1B63C4C-27AD-4E22-8185-5796673CA3AA}"/>
-    <hyperlink ref="R24" r:id="rId5" xr:uid="{08A2F3B9-823C-45C0-969D-0358973D2F16}"/>
+    <hyperlink ref="Q24" r:id="rId5" xr:uid="{08A2F3B9-823C-45C0-969D-0358973D2F16}"/>
     <hyperlink ref="Q29:Q30" r:id="rId6" display="http://purl.obolibrary.org/obo/" xr:uid="{28F37213-D6B5-4C09-8A96-760662AD4884}"/>
     <hyperlink ref="Q29" r:id="rId7" xr:uid="{B0089BD3-5D37-41E4-B827-A728BDB04015}"/>
     <hyperlink ref="Q30" r:id="rId8" xr:uid="{6659EEB8-2061-4ACA-96F4-FD3D15C14968}"/>
-    <hyperlink ref="R26" r:id="rId9" xr:uid="{03F15CA4-4CC8-4E5F-95F9-1B10B541366A}"/>
-    <hyperlink ref="R25" r:id="rId10" xr:uid="{817B7841-B808-4C84-9F77-6406FBC56312}"/>
-    <hyperlink ref="R27" r:id="rId11" xr:uid="{F4AF0096-9932-4C1C-BF5B-FBF5C8F5ACC1}"/>
-    <hyperlink ref="R28" r:id="rId12" xr:uid="{0637E511-30ED-42FB-8DEA-71F67A856866}"/>
+    <hyperlink ref="Q26" r:id="rId9" xr:uid="{03F15CA4-4CC8-4E5F-95F9-1B10B541366A}"/>
+    <hyperlink ref="Q25" r:id="rId10" xr:uid="{817B7841-B808-4C84-9F77-6406FBC56312}"/>
+    <hyperlink ref="Q27" r:id="rId11" xr:uid="{F4AF0096-9932-4C1C-BF5B-FBF5C8F5ACC1}"/>
+    <hyperlink ref="Q28" r:id="rId12" xr:uid="{0637E511-30ED-42FB-8DEA-71F67A856866}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>
@@ -1844,12 +1846,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -1866,7 +1868,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
upgrade templace and converting script
</commit_message>
<xml_diff>
--- a/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
+++ b/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/ToxRSCat/templates/mass_spec_metabolomics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/mass_spec_metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{068CA00F-B5AB-C34E-9C32-7FCEFDD8A366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1ABDF05D-7DA1-426E-9F66-51F463278781}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D160DF7D-B7BB-FC4D-9BE2-4E42D6636DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_description" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="153">
   <si>
     <t>description</t>
   </si>
@@ -519,6 +519,12 @@
   </si>
   <si>
     <t>AUC;nmol/mg protein</t>
+  </si>
+  <si>
+    <t>experiement template version</t>
+  </si>
+  <si>
+    <t>sample template version</t>
   </si>
 </sst>
 </file>
@@ -581,10 +587,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -921,16 +935,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96260E22-F585-4F6B-97AE-516A681FD0BF}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -947,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>83</v>
       </c>
@@ -976,20 +990,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="139" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" style="4" customWidth="1"/>
     <col min="2" max="16" width="21" style="4" customWidth="1"/>
-    <col min="17" max="17" width="32.125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="32.1640625" style="4" customWidth="1"/>
     <col min="18" max="18" width="32" style="4" customWidth="1"/>
-    <col min="19" max="16384" width="11" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -1045,7 +1058,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
@@ -1067,14 +1080,14 @@
       <c r="P2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="170" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1100,11 +1113,11 @@
         <v>1</v>
       </c>
       <c r="Q3" s="3"/>
-      <c r="R3" t="s">
+      <c r="R3" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="170" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
@@ -1128,12 +1141,12 @@
       <c r="O4" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R4" t="s">
+      <c r="R4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="S4" s="3"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S4" s="1"/>
+    </row>
+    <row r="5" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -1162,11 +1175,11 @@
         <v>1</v>
       </c>
       <c r="Q5" s="3"/>
-      <c r="R5" t="s">
+      <c r="R5" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1188,14 +1201,14 @@
       <c r="P6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q6" s="5" t="s">
+      <c r="Q6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R6" t="s">
+      <c r="R6" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>33</v>
       </c>
@@ -1217,14 +1230,14 @@
       <c r="P7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Q7" s="5" t="s">
+      <c r="Q7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R7" t="s">
+      <c r="R7" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="136" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
@@ -1234,7 +1247,7 @@
       <c r="C8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="L8" s="4" t="s">
@@ -1246,12 +1259,11 @@
       <c r="P8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R8"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:19" ht="204" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>33</v>
       </c>
@@ -1270,11 +1282,11 @@
       <c r="O9" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -1293,11 +1305,11 @@
       <c r="N10" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R10" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="404" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
@@ -1310,12 +1322,11 @@
       <c r="E11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="R11"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
@@ -1334,9 +1345,8 @@
       <c r="L12" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="R12"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
@@ -1352,11 +1362,11 @@
       <c r="L13" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="R13" t="s">
+      <c r="R13" s="4" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -1375,11 +1385,11 @@
       <c r="O14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R14" t="s">
+      <c r="R14" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -1398,9 +1408,8 @@
       <c r="N15" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R15"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
@@ -1419,11 +1428,11 @@
       <c r="O16" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R16" t="s">
+      <c r="R16" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" ht="356" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
@@ -1439,11 +1448,11 @@
       <c r="L17" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="R17" t="s">
+      <c r="R17" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
@@ -1459,9 +1468,8 @@
       <c r="L18" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="R18"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>33</v>
       </c>
@@ -1477,9 +1485,8 @@
       <c r="L19" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="R19"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
@@ -1495,11 +1502,11 @@
       <c r="L20" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="R20" t="s">
+      <c r="R20" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" ht="187" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>33</v>
       </c>
@@ -1518,11 +1525,11 @@
       <c r="O21" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R21" t="s">
+      <c r="R21" s="4" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -1541,9 +1548,8 @@
       <c r="N22" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R22"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>33</v>
       </c>
@@ -1562,9 +1568,9 @@
       <c r="L23" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="R23" s="2"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R23" s="6"/>
+    </row>
+    <row r="24" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>33</v>
       </c>
@@ -1589,12 +1595,11 @@
       <c r="P24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q24" s="5" t="s">
+      <c r="Q24" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R24"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
@@ -1616,12 +1621,11 @@
       <c r="P25" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="Q25" s="5" t="s">
+      <c r="Q25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R25"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
@@ -1634,21 +1638,20 @@
       <c r="E26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K26"/>
       <c r="L26" s="4" t="s">
         <v>112</v>
       </c>
       <c r="P26" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="Q26" s="5" t="s">
+      <c r="Q26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R26" t="s">
+      <c r="R26" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>33</v>
       </c>
@@ -1661,7 +1664,7 @@
       <c r="E27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K27" s="4" t="s">
         <v>130</v>
       </c>
       <c r="L27" s="4" t="s">
@@ -1670,14 +1673,14 @@
       <c r="P27" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="Q27" s="5" t="s">
+      <c r="Q27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R27" t="s">
+      <c r="R27" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" ht="272" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>33</v>
       </c>
@@ -1691,7 +1694,7 @@
       <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K28" t="s">
+      <c r="K28" s="4" t="s">
         <v>131</v>
       </c>
       <c r="L28" s="4" t="s">
@@ -1700,14 +1703,14 @@
       <c r="P28" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="Q28" s="5" t="s">
+      <c r="Q28" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R28" t="s">
+      <c r="R28" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
@@ -1726,14 +1729,14 @@
       <c r="P29" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="Q29" s="5" t="s">
+      <c r="Q29" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R29" t="s">
+      <c r="R29" s="4" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
@@ -1752,12 +1755,11 @@
       <c r="P30" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Q30" s="5" t="s">
+      <c r="Q30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R30"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>33</v>
       </c>
@@ -1773,12 +1775,11 @@
       <c r="P31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="Q31" s="5" t="s">
+      <c r="Q31" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R31"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
@@ -1791,11 +1792,11 @@
       <c r="E32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R32" t="s">
+      <c r="R32" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
@@ -1808,9 +1809,8 @@
       <c r="E33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R33"/>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:18" ht="136" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
@@ -1826,9 +1826,8 @@
       <c r="L34" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="R34"/>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:18" ht="187" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -1844,9 +1843,8 @@
       <c r="L35" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="R35"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>33</v>
       </c>
@@ -1859,9 +1857,8 @@
       <c r="E36" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R36"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
@@ -1877,11 +1874,11 @@
       <c r="K37" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="R37" t="s">
+      <c r="R37" s="4" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>73</v>
       </c>
@@ -1900,11 +1897,11 @@
       <c r="O38" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R38" t="s">
+      <c r="R38" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>73</v>
       </c>
@@ -1920,11 +1917,11 @@
       <c r="N39" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R39" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>73</v>
       </c>
@@ -1937,11 +1934,11 @@
       <c r="E40" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R40" t="s">
+      <c r="R40" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>73</v>
       </c>
@@ -1954,11 +1951,11 @@
       <c r="E41" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R41" t="s">
+      <c r="R41" s="4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>73</v>
       </c>
@@ -1971,11 +1968,11 @@
       <c r="E42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R42">
+      <c r="R42" s="4">
         <v>809.12578399999995</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>73</v>
       </c>
@@ -1988,17 +1985,20 @@
       <c r="E43" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R43">
+      <c r="R43" s="4">
         <v>1.23</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>149</v>
       </c>
+      <c r="C44" s="4" t="s">
+        <v>151</v>
+      </c>
       <c r="E44" s="4" t="s">
         <v>149</v>
       </c>
@@ -2006,12 +2006,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>73</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>149</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
update provenance and change the locations of typeof and enums
</commit_message>
<xml_diff>
--- a/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
+++ b/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/mass_spec_metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D160DF7D-B7BB-FC4D-9BE2-4E42D6636DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CFCC00-96FB-0843-AEFC-4E9F2D9364CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_description" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="154">
   <si>
     <t>description</t>
   </si>
@@ -525,6 +525,9 @@
   </si>
   <si>
     <t>sample template version</t>
+  </si>
+  <si>
+    <t>Provenance</t>
   </si>
 </sst>
 </file>
@@ -991,7 +994,7 @@
   <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="139" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2000,7 +2003,7 @@
         <v>151</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="O44" s="4" t="b">
         <v>1</v>
@@ -2017,7 +2020,7 @@
         <v>152</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="O45" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
update readme file, update code and schema based on the updated readme file
</commit_message>
<xml_diff>
--- a/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
+++ b/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/mass_spec_metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00A5B19-197A-1D4A-BEE6-D8A65241CACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05740162-8B88-2E4D-B3A0-24BB39E09989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_description" sheetId="2" r:id="rId1"/>
@@ -573,7 +573,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -581,12 +581,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -602,6 +622,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -993,104 +1029,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="63" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" style="4" customWidth="1"/>
-    <col min="2" max="16" width="21" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="4" customWidth="1"/>
+    <col min="4" max="16" width="21" style="4" customWidth="1"/>
     <col min="17" max="17" width="32.1640625" style="4" customWidth="1"/>
     <col min="18" max="18" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="119" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" s="4" t="b">
+      <c r="C2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="M2" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="170" x14ac:dyDescent="0.2">
+      <c r="N2" s="11"/>
+      <c r="O2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>33</v>
       </c>
@@ -1098,26 +1143,25 @@
         <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
       <c r="L3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N3" s="3"/>
+        <v>67</v>
+      </c>
       <c r="O3" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q3" s="3"/>
+      <c r="P3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="R3" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="170" x14ac:dyDescent="0.2">
@@ -1128,7 +1172,7 @@
         <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>23</v>
@@ -1139,17 +1183,18 @@
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
       <c r="L4" s="4" t="s">
-        <v>90</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="N4" s="3"/>
       <c r="O4" s="4" t="b">
         <v>1</v>
       </c>
+      <c r="Q4" s="3"/>
       <c r="R4" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="5" spans="1:19" ht="102" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="170" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>33</v>
       </c>
@@ -1157,7 +1202,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>153</v>
+        <v>86</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>23</v>
@@ -1168,21 +1213,17 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="M5" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="N5" s="3"/>
+        <v>90</v>
+      </c>
       <c r="O5" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="Q5" s="3"/>
       <c r="R5" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="409.6" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+      <c r="S5" s="1"/>
+    </row>
+    <row r="6" spans="1:19" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
@@ -1654,7 +1695,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>33</v>
       </c>
@@ -1881,156 +1922,257 @@
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="38" spans="1:18" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="M38" s="4" t="b">
+      <c r="D38" s="9"/>
+      <c r="E38" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="O38" s="4" t="b">
+      <c r="N38" s="9"/>
+      <c r="O38" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="R38" s="4" t="s">
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="C39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N39" s="4" t="b">
+      <c r="D39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="R39" s="4" t="s">
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="40" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
+    <row r="40" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E40" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R40" s="4" t="s">
+      <c r="D40" s="7"/>
+      <c r="E40" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A41" s="4" t="s">
+    <row r="41" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R41" s="4" t="s">
+      <c r="D41" s="7"/>
+      <c r="E41" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R42" s="4">
+      <c r="D42" s="7"/>
+      <c r="E42" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7">
         <v>809.12578399999995</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="R43" s="4">
+      <c r="D43" s="7"/>
+      <c r="E43" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7">
         <v>1.23</v>
       </c>
     </row>
-    <row r="44" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="4" t="s">
+    <row r="44" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="D44" s="7"/>
+      <c r="E44" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="O44" s="4" t="b">
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="4" t="s">
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+    </row>
+    <row r="45" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C45" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="D45" s="7"/>
+      <c r="E45" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="O45" s="4" t="b">
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7" t="b">
         <v>1</v>
       </c>
+      <c r="P45" s="7"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Q6:Q8" r:id="rId1" display="http://purl.obolibrary.org/obo/" xr:uid="{4060DE50-60AB-401F-954D-1314EDCB624C}"/>
     <hyperlink ref="Q31" r:id="rId2" xr:uid="{33297E6C-E637-4D6A-A0BC-581B2507D525}"/>
-    <hyperlink ref="Q2" r:id="rId3" xr:uid="{C1B63C4C-27AD-4E22-8185-5796673CA3AA}"/>
+    <hyperlink ref="Q3" r:id="rId3" xr:uid="{C1B63C4C-27AD-4E22-8185-5796673CA3AA}"/>
     <hyperlink ref="Q24" r:id="rId4" xr:uid="{08A2F3B9-823C-45C0-969D-0358973D2F16}"/>
     <hyperlink ref="Q29:Q30" r:id="rId5" display="http://purl.obolibrary.org/obo/" xr:uid="{28F37213-D6B5-4C09-8A96-760662AD4884}"/>
     <hyperlink ref="Q29" r:id="rId6" xr:uid="{B0089BD3-5D37-41E4-B827-A728BDB04015}"/>

</xml_diff>

<commit_message>
add export to mass spec
</commit_message>
<xml_diff>
--- a/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
+++ b/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/mass_spec_metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05740162-8B88-2E4D-B3A0-24BB39E09989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B230523F-BF09-A749-8CB0-EEDFBEE94946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_description" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="160">
   <si>
     <t>description</t>
   </si>
@@ -528,6 +528,24 @@
   </si>
   <si>
     <t>metabolomic_experiment_identifier</t>
+  </si>
+  <si>
+    <t>data_analysis_id</t>
+  </si>
+  <si>
+    <t>metabolite.data_analysis_id</t>
+  </si>
+  <si>
+    <t>chromatography.name</t>
+  </si>
+  <si>
+    <t>name of chromatography</t>
+  </si>
+  <si>
+    <t>ms_method.name</t>
+  </si>
+  <si>
+    <t>name of ms_method</t>
   </si>
 </sst>
 </file>
@@ -606,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -622,10 +640,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -638,6 +652,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1027,10 +1048,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
-  <dimension ref="A1:S45"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1043,63 +1066,63 @@
     <col min="18" max="18" width="32" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:19" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="13" t="s">
+      <c r="L1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="13" t="s">
+      <c r="M1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="O1" s="13" t="s">
+      <c r="N1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="13" t="s">
+      <c r="R1" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>33</v>
       </c>
@@ -1114,23 +1137,21 @@
         <v>23</v>
       </c>
       <c r="F2" s="5"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
       <c r="L2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="N2" s="11"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="9"/>
       <c r="O2" s="5" t="b">
         <v>1</v>
       </c>
       <c r="P2" s="5"/>
-      <c r="Q2" s="11"/>
+      <c r="Q2" s="9"/>
       <c r="R2" s="5" t="s">
         <v>94</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="68" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -1418,22 +1439,22 @@
         <v>61</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>68</v>
+        <v>156</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>97</v>
+        <v>157</v>
       </c>
       <c r="O14" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="R14" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" ht="85" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>33</v>
       </c>
@@ -1441,19 +1462,22 @@
         <v>61</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>23</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="N15" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="O15" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
@@ -1461,42 +1485,42 @@
         <v>61</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="N16" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="E17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="O16" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R16" s="4" t="s">
+      <c r="O17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R17" s="4" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="356" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="R17" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="356" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>33</v>
       </c>
@@ -1504,33 +1528,36 @@
         <v>49</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" s="4" t="s">
+      <c r="E19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="51" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
@@ -1538,42 +1565,36 @@
         <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" s="4" t="s">
+      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="R21" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="187" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="O21" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R21" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -1581,69 +1602,65 @@
         <v>70</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="187" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="O23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L22" s="4" t="s">
+      <c r="E24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="N22" s="4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="68" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="R23" s="6"/>
-    </row>
-    <row r="24" spans="1:18" ht="51" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="O24" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q24" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="N24" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
@@ -1651,25 +1668,20 @@
         <v>35</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>113</v>
+        <v>36</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>27</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q25" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="R25" s="6"/>
+    </row>
+    <row r="26" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
@@ -1677,25 +1689,28 @@
         <v>35</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="O26" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="P26" s="4" t="s">
-        <v>112</v>
+        <v>38</v>
       </c>
       <c r="Q26" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R26" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>33</v>
       </c>
@@ -1703,28 +1718,25 @@
         <v>35</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="R27" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" ht="272" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:18" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>33</v>
       </c>
@@ -1732,76 +1744,82 @@
         <v>35</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>110</v>
+      </c>
       <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="L28" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="K29" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="L29" s="4" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="P29" s="4" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>26</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="272" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>99</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="K30" s="4" t="s">
+        <v>130</v>
+      </c>
       <c r="L30" s="4" t="s">
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="P30" s="4" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="R30" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="31" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
@@ -1811,19 +1829,18 @@
         <v>39</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>43</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="E31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="P31" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q31" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="O31" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" s="6"/>
+    </row>
+    <row r="32" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
@@ -1831,16 +1848,25 @@
         <v>39</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>21</v>
+        <v>96</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="L32" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="P32" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q32" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="R32" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="85" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>33</v>
       </c>
@@ -1848,13 +1874,22 @@
         <v>39</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" ht="136" x14ac:dyDescent="0.2">
+      <c r="L33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q33" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
@@ -1862,16 +1897,19 @@
         <v>39</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L34" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="187" x14ac:dyDescent="0.2">
+      <c r="P34" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q34" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>33</v>
       </c>
@@ -1879,13 +1917,13 @@
         <v>39</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L35" s="4" t="s">
-        <v>124</v>
+      <c r="R35" s="4" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -1896,13 +1934,13 @@
         <v>39</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" ht="136" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
@@ -1910,115 +1948,67 @@
         <v>39</v>
       </c>
       <c r="C37" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L37" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="187" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K37" s="4" t="s">
+      <c r="E40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="R37" s="4" t="s">
+      <c r="R40" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="38" spans="1:18" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="7"/>
-      <c r="N39" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="O39" s="7"/>
-      <c r="P39" s="7"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="7"/>
-      <c r="M40" s="7"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="7"/>
-      <c r="R40" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>73</v>
       </c>
@@ -2026,7 +2016,7 @@
         <v>77</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="7" t="s">
@@ -2039,149 +2029,187 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
       <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
+      <c r="M41" s="7" t="b">
+        <v>1</v>
+      </c>
       <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
+      <c r="O41" s="7" t="b">
+        <v>1</v>
+      </c>
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A42" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
+      <c r="L42" s="14"/>
+      <c r="M42" s="14"/>
+      <c r="N42" s="14"/>
+      <c r="O42" s="14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P42" s="14"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+    </row>
+    <row r="43" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N43" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="R43" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R44" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R45" s="4" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+    <row r="46" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B46" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C46" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7">
+      <c r="E46" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R46" s="4">
         <v>809.12578399999995</v>
       </c>
     </row>
-    <row r="43" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+    <row r="47" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B47" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C47" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="7"/>
-      <c r="Q43" s="7"/>
-      <c r="R43" s="7">
+      <c r="E47" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R47" s="4">
         <v>1.23</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A44" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B44" s="7" t="s">
+    <row r="48" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C48" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7" t="s">
+      <c r="E48" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-    </row>
-    <row r="45" spans="1:18" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="O48" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B49" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C49" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="7"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="P45" s="7"/>
-      <c r="Q45" s="7"/>
-      <c r="R45" s="7"/>
+      <c r="E49" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O49" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="Q6:Q8" r:id="rId1" display="http://purl.obolibrary.org/obo/" xr:uid="{4060DE50-60AB-401F-954D-1314EDCB624C}"/>
-    <hyperlink ref="Q31" r:id="rId2" xr:uid="{33297E6C-E637-4D6A-A0BC-581B2507D525}"/>
+    <hyperlink ref="Q34" r:id="rId2" xr:uid="{33297E6C-E637-4D6A-A0BC-581B2507D525}"/>
     <hyperlink ref="Q3" r:id="rId3" xr:uid="{C1B63C4C-27AD-4E22-8185-5796673CA3AA}"/>
-    <hyperlink ref="Q24" r:id="rId4" xr:uid="{08A2F3B9-823C-45C0-969D-0358973D2F16}"/>
-    <hyperlink ref="Q29:Q30" r:id="rId5" display="http://purl.obolibrary.org/obo/" xr:uid="{28F37213-D6B5-4C09-8A96-760662AD4884}"/>
-    <hyperlink ref="Q29" r:id="rId6" xr:uid="{B0089BD3-5D37-41E4-B827-A728BDB04015}"/>
-    <hyperlink ref="Q30" r:id="rId7" xr:uid="{6659EEB8-2061-4ACA-96F4-FD3D15C14968}"/>
-    <hyperlink ref="Q26" r:id="rId8" xr:uid="{03F15CA4-4CC8-4E5F-95F9-1B10B541366A}"/>
-    <hyperlink ref="Q25" r:id="rId9" xr:uid="{817B7841-B808-4C84-9F77-6406FBC56312}"/>
-    <hyperlink ref="Q27" r:id="rId10" xr:uid="{F4AF0096-9932-4C1C-BF5B-FBF5C8F5ACC1}"/>
-    <hyperlink ref="Q28" r:id="rId11" xr:uid="{0637E511-30ED-42FB-8DEA-71F67A856866}"/>
-    <hyperlink ref="R23:R24" r:id="rId12" display="http://purl.obolibrary.org/obo/" xr:uid="{CCE17E6C-30C2-41DB-9DAC-0DC9C980121B}"/>
+    <hyperlink ref="Q26" r:id="rId4" xr:uid="{08A2F3B9-823C-45C0-969D-0358973D2F16}"/>
+    <hyperlink ref="Q32:Q33" r:id="rId5" display="http://purl.obolibrary.org/obo/" xr:uid="{28F37213-D6B5-4C09-8A96-760662AD4884}"/>
+    <hyperlink ref="Q32" r:id="rId6" xr:uid="{B0089BD3-5D37-41E4-B827-A728BDB04015}"/>
+    <hyperlink ref="Q33" r:id="rId7" xr:uid="{6659EEB8-2061-4ACA-96F4-FD3D15C14968}"/>
+    <hyperlink ref="Q28" r:id="rId8" xr:uid="{03F15CA4-4CC8-4E5F-95F9-1B10B541366A}"/>
+    <hyperlink ref="Q27" r:id="rId9" xr:uid="{817B7841-B808-4C84-9F77-6406FBC56312}"/>
+    <hyperlink ref="Q29" r:id="rId10" xr:uid="{F4AF0096-9932-4C1C-BF5B-FBF5C8F5ACC1}"/>
+    <hyperlink ref="Q30" r:id="rId11" xr:uid="{0637E511-30ED-42FB-8DEA-71F67A856866}"/>
+    <hyperlink ref="R25:R26" r:id="rId12" display="http://purl.obolibrary.org/obo/" xr:uid="{CCE17E6C-30C2-41DB-9DAC-0DC9C980121B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId13"/>

</xml_diff>

<commit_message>
update based on gen3
</commit_message>
<xml_diff>
--- a/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
+++ b/templates/mass_spec_metabolomics/mass_spec_MS_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/ToxRSCat/templates/mass_spec_metabolomics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B230523F-BF09-A749-8CB0-EEDFBEE94946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0047DD5F-5F28-2D42-943D-ABC2F6DDDAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
@@ -329,12 +329,6 @@
     <t>sample_identifier</t>
   </si>
   <si>
-    <t>investigation_identifier</t>
-  </si>
-  <si>
-    <t>study_identifier</t>
-  </si>
-  <si>
     <t>purpose</t>
   </si>
   <si>
@@ -546,6 +540,12 @@
   </si>
   <si>
     <t>name of ms_method</t>
+  </si>
+  <si>
+    <t>program.name</t>
+  </si>
+  <si>
+    <t>project.code</t>
   </si>
 </sst>
 </file>
@@ -624,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -652,13 +652,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1051,9 +1047,10 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="64" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1130,7 +1127,7 @@
         <v>56</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5" t="s">
@@ -1153,7 +1150,7 @@
       <c r="P2" s="5"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="119" x14ac:dyDescent="0.2">
@@ -1164,7 +1161,7 @@
         <v>56</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>87</v>
+        <v>158</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>23</v>
@@ -1182,7 +1179,7 @@
         <v>26</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="170" x14ac:dyDescent="0.2">
@@ -1193,7 +1190,7 @@
         <v>56</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>23</v>
@@ -1212,7 +1209,7 @@
       </c>
       <c r="Q4" s="3"/>
       <c r="R4" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="170" x14ac:dyDescent="0.2">
@@ -1234,13 +1231,13 @@
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="O5" s="4" t="b">
         <v>1</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="S5" s="1"/>
     </row>
@@ -1252,7 +1249,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>23</v>
@@ -1281,7 +1278,7 @@
         <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>23</v>
@@ -1299,7 +1296,7 @@
         <v>26</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="136" x14ac:dyDescent="0.2">
@@ -1342,13 +1339,13 @@
         <v>23</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O9" s="4" t="b">
         <v>1</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="85" x14ac:dyDescent="0.2">
@@ -1365,13 +1362,13 @@
         <v>23</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N10" s="4" t="b">
         <v>1</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="404" x14ac:dyDescent="0.2">
@@ -1388,7 +1385,7 @@
         <v>27</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
@@ -1405,10 +1402,10 @@
         <v>27</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="68" x14ac:dyDescent="0.2">
@@ -1425,10 +1422,10 @@
         <v>23</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="34" x14ac:dyDescent="0.2">
@@ -1439,7 +1436,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>13</v>
@@ -1448,7 +1445,7 @@
         <v>23</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="O14" s="4" t="b">
         <v>1</v>
@@ -1468,13 +1465,13 @@
         <v>23</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O15" s="4" t="b">
         <v>1</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="85" x14ac:dyDescent="0.2">
@@ -1491,7 +1488,7 @@
         <v>23</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N16" s="4" t="b">
         <v>1</v>
@@ -1517,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="356" x14ac:dyDescent="0.2">
@@ -1534,10 +1531,10 @@
         <v>23</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="68" x14ac:dyDescent="0.2">
@@ -1554,7 +1551,7 @@
         <v>23</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:18" ht="51" x14ac:dyDescent="0.2">
@@ -1571,7 +1568,7 @@
         <v>23</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="68" x14ac:dyDescent="0.2">
@@ -1588,10 +1585,10 @@
         <v>23</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -1602,7 +1599,7 @@
         <v>70</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>13</v>
@@ -1614,7 +1611,7 @@
         <v>1</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="187" x14ac:dyDescent="0.2">
@@ -1631,13 +1628,13 @@
         <v>23</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="O23" s="4" t="b">
         <v>1</v>
       </c>
       <c r="R23" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="85" x14ac:dyDescent="0.2">
@@ -1654,7 +1651,7 @@
         <v>23</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="N24" s="4" t="b">
         <v>1</v>
@@ -1674,10 +1671,10 @@
         <v>27</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="R25" s="6"/>
     </row>
@@ -1698,7 +1695,7 @@
         <v>65</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="O26" s="4" t="b">
         <v>1</v>
@@ -1718,19 +1715,19 @@
         <v>35</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>27</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P27" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="Q27" s="6" t="s">
         <v>26</v>
@@ -1744,22 +1741,22 @@
         <v>35</v>
       </c>
       <c r="C28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="P28" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="P28" s="4" t="s">
-        <v>112</v>
       </c>
       <c r="Q28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="409.6" x14ac:dyDescent="0.2">
@@ -1770,25 +1767,25 @@
         <v>35</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="P29" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P29" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="Q29" s="6" t="s">
         <v>26</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="272" x14ac:dyDescent="0.2">
@@ -1799,26 +1796,26 @@
         <v>35</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="4" t="s">
         <v>23</v>
       </c>
       <c r="K30" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L30" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="P30" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="P30" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="Q30" s="6" t="s">
         <v>26</v>
       </c>
       <c r="R30" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -1829,7 +1826,7 @@
         <v>39</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="4" t="s">
@@ -1848,22 +1845,22 @@
         <v>39</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L32" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="P32" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="P32" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="Q32" s="6" t="s">
         <v>26</v>
       </c>
       <c r="R32" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="85" x14ac:dyDescent="0.2">
@@ -1874,16 +1871,16 @@
         <v>39</v>
       </c>
       <c r="C33" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="P33" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="P33" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="Q33" s="6" t="s">
         <v>26</v>
@@ -1923,7 +1920,7 @@
         <v>23</v>
       </c>
       <c r="R35" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -1954,7 +1951,7 @@
         <v>23</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="187" x14ac:dyDescent="0.2">
@@ -1971,7 +1968,7 @@
         <v>23</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2002,10 +1999,10 @@
         <v>23</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="R40" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -2039,40 +2036,28 @@
       <c r="P41" s="7"/>
       <c r="Q41" s="7"/>
       <c r="R41" s="7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" s="15" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
         <v>73</v>
       </c>
       <c r="B42" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C42" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
-      <c r="L42" s="14"/>
-      <c r="M42" s="14"/>
-      <c r="N42" s="14"/>
-      <c r="O42" s="14" t="b">
-        <v>1</v>
-      </c>
-      <c r="P42" s="14"/>
-      <c r="Q42" s="14"/>
-      <c r="R42" s="14"/>
+      <c r="C42" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O42" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
@@ -2091,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="R43" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2108,7 +2093,7 @@
         <v>23</v>
       </c>
       <c r="R44" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2125,7 +2110,7 @@
         <v>23</v>
       </c>
       <c r="R45" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="17" x14ac:dyDescent="0.2">
@@ -2167,13 +2152,13 @@
         <v>33</v>
       </c>
       <c r="B48" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="O48" s="4" t="b">
         <v>1</v>
@@ -2184,10 +2169,10 @@
         <v>73</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>23</v>

</xml_diff>